<commit_message>
feat: add new template strings to quotation generation
</commit_message>
<xml_diff>
--- a/backend/src/Templates/cotizacion_plantilla.xlsx
+++ b/backend/src/Templates/cotizacion_plantilla.xlsx
@@ -211,7 +211,7 @@
     <t xml:space="preserve">{{forma_pago}}</t>
   </si>
   <si>
-    <t xml:space="preserve">Trabajos Diurnos </t>
+    <t xml:space="preserve">{{otros}}</t>
   </si>
   <si>
     <t xml:space="preserve">Cantidad</t>
@@ -279,7 +279,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">1.- Los precios </t>
+      <t xml:space="preserve">1.- Los precios</t>
     </r>
     <r>
       <rPr>
@@ -289,7 +289,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">No</t>
+      <t xml:space="preserve"> {{tiene_igv_2}} </t>
     </r>
     <r>
       <rPr>
@@ -298,7 +298,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> Incluyen IGV</t>
+      <t xml:space="preserve">Incluyen IGV</t>
     </r>
   </si>
   <si>
@@ -1266,7 +1266,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="3" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1514,9 +1514,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>159840</xdr:colOff>
+      <xdr:colOff>159480</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1386000</xdr:rowOff>
+      <xdr:rowOff>1385640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1530,7 +1530,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="91440"/>
-          <a:ext cx="10590480" cy="1294560"/>
+          <a:ext cx="10590120" cy="1294200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1552,9 +1552,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>79560</xdr:colOff>
+      <xdr:colOff>79200</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1446840</xdr:rowOff>
+      <xdr:rowOff>1446480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1564,7 +1564,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7388640" y="674280"/>
-          <a:ext cx="3121560" cy="772560"/>
+          <a:ext cx="3121200" cy="772200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1619,9 +1619,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>281160</xdr:colOff>
+      <xdr:colOff>280800</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1132920</xdr:rowOff>
+      <xdr:rowOff>1132560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1631,7 +1631,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="152280" y="381600"/>
-          <a:ext cx="5918760" cy="751320"/>
+          <a:ext cx="5918400" cy="750960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1708,9 +1708,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>321480</xdr:colOff>
+      <xdr:colOff>321120</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:rowOff>2880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1724,7 +1724,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4614120" y="0"/>
-          <a:ext cx="1497240" cy="1451160"/>
+          <a:ext cx="1496880" cy="1450800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1749,9 +1749,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>157320</xdr:colOff>
+      <xdr:colOff>156960</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>253080</xdr:rowOff>
+      <xdr:rowOff>252720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1765,7 +1765,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="14714280"/>
-          <a:ext cx="10587960" cy="933120"/>
+          <a:ext cx="10587600" cy="932760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1787,9 +1787,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1440</xdr:colOff>
+      <xdr:colOff>1080</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>175320</xdr:rowOff>
+      <xdr:rowOff>174960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1799,7 +1799,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="14640840"/>
-          <a:ext cx="10591920" cy="928800"/>
+          <a:ext cx="10591560" cy="928440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1953,9 +1953,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4285440</xdr:colOff>
+      <xdr:colOff>4285080</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>261360</xdr:rowOff>
+      <xdr:rowOff>261000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1969,7 +1969,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2679480" y="12562200"/>
-          <a:ext cx="2317320" cy="1436040"/>
+          <a:ext cx="2316960" cy="1435680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1991,9 +1991,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>969120</xdr:colOff>
+      <xdr:colOff>968760</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>307800</xdr:rowOff>
+      <xdr:rowOff>307440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2007,7 +2007,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5848200" y="12736440"/>
-          <a:ext cx="2128680" cy="976680"/>
+          <a:ext cx="2128320" cy="976320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2225,8 +2225,8 @@
   </sheetPr>
   <dimension ref="B1:H39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.78125" defaultRowHeight="26.1" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>